<commit_message>
Fixed a few errors in Snake_River_TRT_Populations.xlsx. Minor additions to results and conclusions of TrapRateEffects.Rmd
</commit_message>
<xml_diff>
--- a/data/Snake_River_TRT_Populations.xlsx
+++ b/data/Snake_River_TRT_Populations.xlsx
@@ -3,24 +3,30 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4DB8E78-DDFB-49CA-99C3-D4D5217C58B3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6AE7B42-5774-4113-8DBF-5154B443E95E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="125">
   <si>
     <t>Species</t>
   </si>
@@ -121,9 +127,6 @@
     <t>Big Sheep Creek</t>
   </si>
   <si>
-    <t>Little Salmon</t>
-  </si>
-  <si>
     <t>SRLSR</t>
   </si>
   <si>
@@ -166,9 +169,6 @@
     <t>MFLOO</t>
   </si>
   <si>
-    <t>MFPIS</t>
-  </si>
-  <si>
     <t>MFSUL</t>
   </si>
   <si>
@@ -193,9 +193,6 @@
     <t>Loon Creek</t>
   </si>
   <si>
-    <t>Pistol Creek</t>
-  </si>
-  <si>
     <t>Sulphur Creek</t>
   </si>
   <si>
@@ -358,9 +355,6 @@
     <t>MFUMA-s</t>
   </si>
   <si>
-    <t>MFPAN-s</t>
-  </si>
-  <si>
     <t>SRNFS-s</t>
   </si>
   <si>
@@ -404,13 +398,23 @@
   </si>
   <si>
     <t>Hells Canyon tributaries</t>
+  </si>
+  <si>
+    <t>SRPAN-s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -436,14 +440,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 10" xfId="1" xr:uid="{F42E2042-5ED0-40FB-AADD-5D3219D4C3E3}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -721,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -750,7 +756,7 @@
         <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -761,13 +767,13 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -778,13 +784,13 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -795,13 +801,13 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -812,13 +818,13 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -829,13 +835,13 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D6" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -846,13 +852,13 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D7" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -863,13 +869,13 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="D8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -880,13 +886,13 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -897,13 +903,13 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -914,13 +920,13 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -931,13 +937,13 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -948,13 +954,13 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D13" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -965,13 +971,13 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D14" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E14" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -982,13 +988,13 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D15" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -999,13 +1005,13 @@
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D16" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1016,13 +1022,13 @@
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E17" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1033,13 +1039,13 @@
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D18" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1050,13 +1056,13 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D19" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E19" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1067,13 +1073,13 @@
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D20" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E20" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1084,13 +1090,13 @@
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D21" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E21" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1101,13 +1107,13 @@
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D22" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E22" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1118,13 +1124,13 @@
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D23" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E23" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1135,13 +1141,13 @@
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D24" t="s">
         <v>30</v>
       </c>
       <c r="E24" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1149,13 +1155,13 @@
         <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C25" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D25" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E25" t="s">
         <v>79</v>
@@ -1169,13 +1175,13 @@
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D26" t="s">
         <v>16</v>
       </c>
       <c r="E26" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1186,13 +1192,13 @@
         <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D27" t="s">
         <v>18</v>
       </c>
       <c r="E27" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1203,13 +1209,13 @@
         <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D28" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E28" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1220,13 +1226,13 @@
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D29" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E29" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1237,13 +1243,13 @@
         <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D30" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E30" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1254,13 +1260,13 @@
         <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D31" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E31" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1271,13 +1277,13 @@
         <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D32" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E32" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1288,13 +1294,13 @@
         <v>10</v>
       </c>
       <c r="C33" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D33" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E33" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1305,13 +1311,13 @@
         <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D34" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E34" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1322,13 +1328,13 @@
         <v>10</v>
       </c>
       <c r="C35" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D35" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E35" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1339,13 +1345,13 @@
         <v>10</v>
       </c>
       <c r="C36" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D36" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E36" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1356,13 +1362,13 @@
         <v>11</v>
       </c>
       <c r="C37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D37" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E37" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -1373,13 +1379,13 @@
         <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D38" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E38" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1390,13 +1396,13 @@
         <v>11</v>
       </c>
       <c r="C39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D39" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E39" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1407,13 +1413,13 @@
         <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D40" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E40" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1424,13 +1430,13 @@
         <v>11</v>
       </c>
       <c r="C41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D41" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E41" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1441,13 +1447,13 @@
         <v>11</v>
       </c>
       <c r="C42" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D42" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E42" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1458,13 +1464,13 @@
         <v>11</v>
       </c>
       <c r="C43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D43" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E43" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1475,13 +1481,13 @@
         <v>11</v>
       </c>
       <c r="C44" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D44" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E44" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -1492,13 +1498,13 @@
         <v>11</v>
       </c>
       <c r="C45" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D45" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="E45" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -1506,16 +1512,16 @@
         <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="C46" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D46" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E46" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -1532,7 +1538,7 @@
         <v>39</v>
       </c>
       <c r="E47" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -1549,7 +1555,7 @@
         <v>40</v>
       </c>
       <c r="E48" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1560,13 +1566,13 @@
         <v>12</v>
       </c>
       <c r="C49" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D49" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E49" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1574,16 +1580,16 @@
         <v>3</v>
       </c>
       <c r="B50" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C50" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D50" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="E50" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1594,13 +1600,13 @@
         <v>13</v>
       </c>
       <c r="C51" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D51" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E51" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1611,13 +1617,13 @@
         <v>13</v>
       </c>
       <c r="C52" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D52" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E52" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -1628,13 +1634,13 @@
         <v>13</v>
       </c>
       <c r="C53" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D53" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E53" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -1645,13 +1651,13 @@
         <v>13</v>
       </c>
       <c r="C54" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D54" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E54" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -1662,13 +1668,13 @@
         <v>13</v>
       </c>
       <c r="C55" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D55" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E55" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -1679,10 +1685,10 @@
         <v>13</v>
       </c>
       <c r="C56" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D56" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E56" t="s">
         <v>79</v>
@@ -1696,10 +1702,10 @@
         <v>13</v>
       </c>
       <c r="C57" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="D57" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="E57" t="s">
         <v>79</v>
@@ -1710,16 +1716,16 @@
         <v>3</v>
       </c>
       <c r="B58" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C58" t="s">
-        <v>83</v>
+        <v>15</v>
       </c>
       <c r="D58" t="s">
-        <v>84</v>
+        <v>16</v>
       </c>
       <c r="E58" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -1730,29 +1736,12 @@
         <v>9</v>
       </c>
       <c r="C59" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D59" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E59" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>3</v>
-      </c>
-      <c r="B60" t="s">
-        <v>9</v>
-      </c>
-      <c r="C60" t="s">
-        <v>17</v>
-      </c>
-      <c r="D60" t="s">
-        <v>18</v>
-      </c>
-      <c r="E60" t="s">
         <v>79</v>
       </c>
     </row>

</xml_diff>